<commit_message>
XMI from EA Sparx started
</commit_message>
<xml_diff>
--- a/import/generator.xlsx
+++ b/import/generator.xlsx
@@ -1,18 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
-    <sheet name="List2" sheetId="2" r:id="rId2"/>
-    <sheet name="List3" sheetId="3" r:id="rId3"/>
+    <sheet name="Business Processes" sheetId="1" r:id="rId1"/>
+    <sheet name="Applications" sheetId="2" r:id="rId2"/>
+    <sheet name="ID" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ID!$L$2:$O$2</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+  <si>
+    <t>2c19695</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t>HEX</t>
+  </si>
+  <si>
+    <t>Hex Start</t>
+  </si>
+  <si>
+    <t>Dec Start</t>
+  </si>
+  <si>
+    <t>len(HEX)</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Homer Select</t>
+  </si>
+  <si>
+    <t>LDAP  OpenAM</t>
+  </si>
+  <si>
+    <t>Siebel or HomeSIS </t>
+  </si>
+  <si>
+    <t>Home Portal </t>
+  </si>
+  <si>
+    <t>OBI reports</t>
+  </si>
+  <si>
+    <t>BSL</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>LAP</t>
+  </si>
+  <si>
+    <t>WF Designer</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Black&amp;White Lists</t>
+  </si>
+  <si>
+    <t>HomeDW </t>
+  </si>
+  <si>
+    <t>HomeDW</t>
+  </si>
+  <si>
+    <t>Product Management</t>
+  </si>
+  <si>
+    <t>Cabinet</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>CaBus</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>CIF</t>
+  </si>
+  <si>
+    <t>Loxon</t>
+  </si>
+  <si>
+    <t>SAS or Loxon</t>
+  </si>
+  <si>
+    <t>Planned group solution</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -59,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -99,7 +195,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -169,7 +265,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -345,7 +441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -369,13 +467,1258 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>HEX2DEC(B3)</f>
+        <v>46241429</v>
+      </c>
+      <c r="D3" t="str">
+        <f>DEC2HEX(C3)</f>
+        <v>2C19695</v>
+      </c>
+      <c r="G3">
+        <v>46241429</v>
+      </c>
+      <c r="H3" t="str">
+        <f>DEC2HEX(G3)</f>
+        <v>2C19695</v>
+      </c>
+      <c r="I3">
+        <f>LEN(H3)</f>
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <f>HEX2DEC(H3)</f>
+        <v>46241429</v>
+      </c>
+      <c r="L3">
+        <f ca="1">RANDBETWEEN($G$4,$G$5)</f>
+        <v>90178858</v>
+      </c>
+      <c r="M3" t="str">
+        <f ca="1">DEC2HEX(L3)</f>
+        <v>560052A</v>
+      </c>
+      <c r="N3">
+        <f ca="1">LEN(M3)</f>
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <f ca="1">HEX2DEC(M3)</f>
+        <v>90178858</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="G4">
+        <v>22222222</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H29" si="0">DEC2HEX(G4)</f>
+        <v>153158E</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I29" si="1">LEN(H4)</f>
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J29" si="2">HEX2DEC(H4)</f>
+        <v>22222222</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L40" ca="1" si="3">RANDBETWEEN($G$4,$G$5)</f>
+        <v>47679479</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M40" ca="1" si="4">DEC2HEX(L4)</f>
+        <v>2D787F7</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N40" ca="1" si="5">LEN(M4)</f>
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O40" ca="1" si="6">HEX2DEC(M4)</f>
+        <v>47679479</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="G5">
+        <v>99999999</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>5F5E0FF</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>99999999</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="3"/>
+        <v>64802274</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>3DCCDE2</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="6"/>
+        <v>64802274</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="3"/>
+        <v>34720450</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>211CAC2</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="6"/>
+        <v>34720450</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="3"/>
+        <v>41940024</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>27FF438</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="6"/>
+        <v>41940024</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="3"/>
+        <v>54911939</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>345E3C3</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="6"/>
+        <v>54911939</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="3"/>
+        <v>52242939</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>31D29FB</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="6"/>
+        <v>52242939</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="3"/>
+        <v>67472065</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>4058AC1</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="6"/>
+        <v>67472065</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ca="1" si="3"/>
+        <v>74579308</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>471FD6C</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="6"/>
+        <v>74579308</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="3"/>
+        <v>72375884</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>4505E4C</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="6"/>
+        <v>72375884</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="3"/>
+        <v>38460830</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>24ADD9E</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="6"/>
+        <v>38460830</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="3"/>
+        <v>37279629</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>238D78D</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="6"/>
+        <v>37279629</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ca="1" si="3"/>
+        <v>65186488</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>3E2AAB8</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="6"/>
+        <v>65186488</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ca="1" si="3"/>
+        <v>72867766</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>457DFB6</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="6"/>
+        <v>72867766</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15">
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="3"/>
+        <v>69311180</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>4219ACC</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ca="1" si="6"/>
+        <v>69311180</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15">
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="3"/>
+        <v>31834820</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>1E5C2C4</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ca="1" si="6"/>
+        <v>31834820</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15">
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ca="1" si="3"/>
+        <v>91320631</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>5717137</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ca="1" si="6"/>
+        <v>91320631</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15">
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ca="1" si="3"/>
+        <v>39583633</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>25BFF91</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ca="1" si="6"/>
+        <v>39583633</v>
+      </c>
+    </row>
+    <row r="21" spans="8:15">
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ca="1" si="3"/>
+        <v>56406556</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>35CB21C</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ca="1" si="6"/>
+        <v>56406556</v>
+      </c>
+    </row>
+    <row r="22" spans="8:15">
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ca="1" si="3"/>
+        <v>36371482</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>22AFC1A</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ca="1" si="6"/>
+        <v>36371482</v>
+      </c>
+    </row>
+    <row r="23" spans="8:15">
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ca="1" si="3"/>
+        <v>49025968</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>2EC13B0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ca="1" si="6"/>
+        <v>49025968</v>
+      </c>
+    </row>
+    <row r="24" spans="8:15">
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ca="1" si="3"/>
+        <v>23685000</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>1696788</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="6"/>
+        <v>23685000</v>
+      </c>
+    </row>
+    <row r="25" spans="8:15">
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ca="1" si="3"/>
+        <v>95526741</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>5B19F55</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="6"/>
+        <v>95526741</v>
+      </c>
+    </row>
+    <row r="26" spans="8:15">
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="3"/>
+        <v>90076717</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>55E762D</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="6"/>
+        <v>90076717</v>
+      </c>
+    </row>
+    <row r="27" spans="8:15">
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ca="1" si="3"/>
+        <v>71872649</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>448B089</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="6"/>
+        <v>71872649</v>
+      </c>
+    </row>
+    <row r="28" spans="8:15">
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" ca="1" si="3"/>
+        <v>75214625</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>47BAF21</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="6"/>
+        <v>75214625</v>
+      </c>
+    </row>
+    <row r="29" spans="8:15">
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ca="1" si="3"/>
+        <v>24574446</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>176F9EE</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="6"/>
+        <v>24574446</v>
+      </c>
+    </row>
+    <row r="30" spans="8:15">
+      <c r="L30">
+        <f t="shared" ca="1" si="3"/>
+        <v>77315111</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>49BBC27</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="6"/>
+        <v>77315111</v>
+      </c>
+    </row>
+    <row r="31" spans="8:15">
+      <c r="L31">
+        <f t="shared" ca="1" si="3"/>
+        <v>63434622</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>3C7EF7E</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ca="1" si="6"/>
+        <v>63434622</v>
+      </c>
+    </row>
+    <row r="32" spans="8:15">
+      <c r="L32">
+        <f t="shared" ca="1" si="3"/>
+        <v>31716060</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>1E3F2DC</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="6"/>
+        <v>31716060</v>
+      </c>
+    </row>
+    <row r="33" spans="12:15">
+      <c r="L33">
+        <f t="shared" ca="1" si="3"/>
+        <v>90616689</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>566B371</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="6"/>
+        <v>90616689</v>
+      </c>
+    </row>
+    <row r="34" spans="12:15">
+      <c r="L34">
+        <f t="shared" ca="1" si="3"/>
+        <v>40649957</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>26C44E5</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="6"/>
+        <v>40649957</v>
+      </c>
+    </row>
+    <row r="35" spans="12:15">
+      <c r="L35">
+        <f t="shared" ca="1" si="3"/>
+        <v>26274462</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>190EA9E</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ca="1" si="6"/>
+        <v>26274462</v>
+      </c>
+    </row>
+    <row r="36" spans="12:15">
+      <c r="L36">
+        <f t="shared" ca="1" si="3"/>
+        <v>74508442</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>470E89A</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ca="1" si="6"/>
+        <v>74508442</v>
+      </c>
+    </row>
+    <row r="37" spans="12:15">
+      <c r="L37">
+        <f t="shared" ca="1" si="3"/>
+        <v>78134082</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>4A83B42</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O37">
+        <f t="shared" ca="1" si="6"/>
+        <v>78134082</v>
+      </c>
+    </row>
+    <row r="38" spans="12:15">
+      <c r="L38">
+        <f t="shared" ca="1" si="3"/>
+        <v>91962055</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>57B3AC7</v>
+      </c>
+      <c r="N38">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O38">
+        <f t="shared" ca="1" si="6"/>
+        <v>91962055</v>
+      </c>
+    </row>
+    <row r="39" spans="12:15">
+      <c r="L39">
+        <f t="shared" ca="1" si="3"/>
+        <v>55342651</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>34C763B</v>
+      </c>
+      <c r="N39">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ca="1" si="6"/>
+        <v>55342651</v>
+      </c>
+    </row>
+    <row r="40" spans="12:15">
+      <c r="L40">
+        <f t="shared" ca="1" si="3"/>
+        <v>29278183</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>1BEBFE7</v>
+      </c>
+      <c r="N40">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O40">
+        <f t="shared" ca="1" si="6"/>
+        <v>29278183</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="G4:G71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="7:7">
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="7:7">
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="7:7">
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="7:7">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="7:7">
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="7:7">
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="7:7">
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="7:7">
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="7:7">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="7:7">
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="7:7">
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="7:7">
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="7:7">
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7">
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7">
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7">
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7">
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7">
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7">
+      <c r="G35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7">
+      <c r="G45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7">
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7">
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7">
+      <c r="G52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7">
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7">
+      <c r="G54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7">
+      <c r="G55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7">
+      <c r="G57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7">
+      <c r="G64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7">
+      <c r="G69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7">
+      <c r="G71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
XMI from EA: components imported to ARCHI!
</commit_message>
<xml_diff>
--- a/import/generator.xlsx
+++ b/import/generator.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Business Processes" sheetId="1" r:id="rId1"/>
     <sheet name="Applications" sheetId="2" r:id="rId2"/>
     <sheet name="ID" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ID!$L$2:$O$2</definedName>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>2c19695</t>
   </si>
@@ -43,80 +42,530 @@
     <t>Random</t>
   </si>
   <si>
-    <t>Homer Select</t>
-  </si>
-  <si>
-    <t>LDAP  OpenAM</t>
-  </si>
-  <si>
-    <t>Siebel or HomeSIS </t>
-  </si>
-  <si>
-    <t>Home Portal </t>
-  </si>
-  <si>
-    <t>OBI reports</t>
-  </si>
-  <si>
-    <t>BSL</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>LAP</t>
-  </si>
-  <si>
-    <t>WF Designer</t>
-  </si>
-  <si>
-    <t>Blaze</t>
-  </si>
-  <si>
-    <t>Black&amp;White Lists</t>
-  </si>
-  <si>
-    <t>HomeDW </t>
-  </si>
-  <si>
-    <t>HomeDW</t>
-  </si>
-  <si>
-    <t>Product Management</t>
-  </si>
-  <si>
-    <t>Cabinet</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>CaBus</t>
-  </si>
-  <si>
-    <t>Insurance</t>
-  </si>
-  <si>
-    <t>CIF</t>
-  </si>
-  <si>
-    <t>Loxon</t>
-  </si>
-  <si>
-    <t>SAS or Loxon</t>
-  </si>
-  <si>
-    <t>Planned group solution</t>
+    <t xml:space="preserve">          &lt;property key="GUID" value="ABRAKADABRA"/&gt;</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>pro kazdou vyrobit fake function</t>
+  </si>
+  <si>
+    <t>a spojit ji assignment (komponenta to function) relation s aplikacni komponentou</t>
+  </si>
+  <si>
+    <t>. Fake pujde vymazat po napojeni realnych funkci.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. </t>
+  </si>
+  <si>
+    <t>vyrobit jednu aplikacni sluzbu a napojit ji na tu funkci. Vsechny funkce napojim na tuto jednu sluzbu.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>realizuj used by ze Service na Component</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>vyrobit pro kazdou interface a napojit ho na komponentu a Assignment na app service</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;element xsi:type="archimate:archimate:ApplicationComponent" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16a2d67e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Old Homer"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;element xsi:type="archimate:ApplicationFunction" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2ff20be0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Ab"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;element xsi:type="archimate:AssignmentRelationship" id="3afc79bd" name="adas" source="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16a2d67e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" target="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2ff20be0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     &lt;element xsi:type="archimate:ApplicationService" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>748c2283</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Ac"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;element xsi:type="archimate:RealisationRelationship" id="2f6a50b9" name="hudry" source="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2ff20be0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" target="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>748c2283</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;element xsi:type="archimate:ApplicationInterface" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8fa23d6a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Aint"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   &lt;element xsi:type="archimate:CompositionRelationship" id="0a2e9135" name="int" source="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16a2d67e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" target="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8fa23d6a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   &lt;element xsi:type="archimate:AssignmentRelationship" id="7ec37d8d" source="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8fa23d6a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" target="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>748c2283</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;element xsi:type="archimate:ApplicationService" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6e48183a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Bb"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     &lt;element xsi:type="archimate:ApplicationFunction" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2ff20be0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Ab"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;element xsi:type="archimate:UsedByRelationship" id="bb86547f" name="blb" source="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6e48183a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" target="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2ff20be0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>predesle kroky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -143,8 +592,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,12 +904,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -470,7 +1057,7 @@
   <dimension ref="B2:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -545,11 +1132,11 @@
       </c>
       <c r="L3">
         <f ca="1">RANDBETWEEN($G$4,$G$5)</f>
-        <v>90178858</v>
+        <v>99999996</v>
       </c>
       <c r="M3" t="str">
         <f ca="1">DEC2HEX(L3)</f>
-        <v>560052A</v>
+        <v>5F5E0FC</v>
       </c>
       <c r="N3">
         <f ca="1">LEN(M3)</f>
@@ -557,16 +1144,16 @@
       </c>
       <c r="O3">
         <f ca="1">HEX2DEC(M3)</f>
-        <v>90178858</v>
+        <v>99999996</v>
       </c>
     </row>
     <row r="4" spans="2:15">
       <c r="G4">
-        <v>22222222</v>
+        <v>99999000</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ref="H4:H29" si="0">DEC2HEX(G4)</f>
-        <v>153158E</v>
+        <v>5F5DD18</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I29" si="1">LEN(H4)</f>
@@ -574,15 +1161,15 @@
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J29" si="2">HEX2DEC(H4)</f>
-        <v>22222222</v>
+        <v>99999000</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L40" ca="1" si="3">RANDBETWEEN($G$4,$G$5)</f>
-        <v>47679479</v>
+        <v>99999970</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M40" ca="1" si="4">DEC2HEX(L4)</f>
-        <v>2D787F7</v>
+        <v>5F5E0E2</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N40" ca="1" si="5">LEN(M4)</f>
@@ -590,7 +1177,7 @@
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O40" ca="1" si="6">HEX2DEC(M4)</f>
-        <v>47679479</v>
+        <v>99999970</v>
       </c>
     </row>
     <row r="5" spans="2:15">
@@ -611,11 +1198,11 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="3"/>
-        <v>64802274</v>
+        <v>99999489</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>3DCCDE2</v>
+        <v>5F5DF01</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="5"/>
@@ -623,7 +1210,7 @@
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="6"/>
-        <v>64802274</v>
+        <v>99999489</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -641,11 +1228,11 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="3"/>
-        <v>34720450</v>
+        <v>99999570</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>211CAC2</v>
+        <v>5F5DF52</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="5"/>
@@ -653,7 +1240,7 @@
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="6"/>
-        <v>34720450</v>
+        <v>99999570</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -671,11 +1258,11 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="3"/>
-        <v>41940024</v>
+        <v>99999004</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>27FF438</v>
+        <v>5F5DD1C</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="5"/>
@@ -683,7 +1270,7 @@
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="6"/>
-        <v>41940024</v>
+        <v>99999004</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -701,11 +1288,11 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="3"/>
-        <v>54911939</v>
+        <v>99999546</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>345E3C3</v>
+        <v>5F5DF3A</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="5"/>
@@ -713,7 +1300,7 @@
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="6"/>
-        <v>54911939</v>
+        <v>99999546</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -731,11 +1318,11 @@
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="3"/>
-        <v>52242939</v>
+        <v>99999930</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>31D29FB</v>
+        <v>5F5E0BA</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="5"/>
@@ -743,7 +1330,7 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="6"/>
-        <v>52242939</v>
+        <v>99999930</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -761,11 +1348,11 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="3"/>
-        <v>67472065</v>
+        <v>99999407</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>4058AC1</v>
+        <v>5F5DEAF</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="5"/>
@@ -773,7 +1360,7 @@
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="6"/>
-        <v>67472065</v>
+        <v>99999407</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -791,11 +1378,11 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="3"/>
-        <v>74579308</v>
+        <v>99999149</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>471FD6C</v>
+        <v>5F5DDAD</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="5"/>
@@ -803,7 +1390,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="6"/>
-        <v>74579308</v>
+        <v>99999149</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -821,11 +1408,11 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="3"/>
-        <v>72375884</v>
+        <v>99999758</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>4505E4C</v>
+        <v>5F5E00E</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="5"/>
@@ -833,7 +1420,7 @@
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="6"/>
-        <v>72375884</v>
+        <v>99999758</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -851,11 +1438,11 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>38460830</v>
+        <v>99999390</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>24ADD9E</v>
+        <v>5F5DE9E</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="5"/>
@@ -863,7 +1450,7 @@
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="6"/>
-        <v>38460830</v>
+        <v>99999390</v>
       </c>
     </row>
     <row r="14" spans="2:15">
@@ -881,11 +1468,11 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>37279629</v>
+        <v>99999460</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>238D78D</v>
+        <v>5F5DEE4</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="5"/>
@@ -893,7 +1480,7 @@
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="6"/>
-        <v>37279629</v>
+        <v>99999460</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -911,11 +1498,11 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>65186488</v>
+        <v>99999050</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>3E2AAB8</v>
+        <v>5F5DD4A</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="5"/>
@@ -923,7 +1510,7 @@
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="6"/>
-        <v>65186488</v>
+        <v>99999050</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -941,11 +1528,11 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
-        <v>72867766</v>
+        <v>99999668</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>457DFB6</v>
+        <v>5F5DFB4</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="5"/>
@@ -953,7 +1540,7 @@
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="6"/>
-        <v>72867766</v>
+        <v>99999668</v>
       </c>
     </row>
     <row r="17" spans="8:15">
@@ -971,11 +1558,11 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>69311180</v>
+        <v>99999803</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>4219ACC</v>
+        <v>5F5E03B</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="5"/>
@@ -983,7 +1570,7 @@
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="6"/>
-        <v>69311180</v>
+        <v>99999803</v>
       </c>
     </row>
     <row r="18" spans="8:15">
@@ -1001,11 +1588,11 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="3"/>
-        <v>31834820</v>
+        <v>99999289</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1E5C2C4</v>
+        <v>5F5DE39</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="5"/>
@@ -1013,7 +1600,7 @@
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="6"/>
-        <v>31834820</v>
+        <v>99999289</v>
       </c>
     </row>
     <row r="19" spans="8:15">
@@ -1031,11 +1618,11 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>91320631</v>
+        <v>99999024</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5717137</v>
+        <v>5F5DD30</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="5"/>
@@ -1043,7 +1630,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="6"/>
-        <v>91320631</v>
+        <v>99999024</v>
       </c>
     </row>
     <row r="20" spans="8:15">
@@ -1061,11 +1648,11 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="3"/>
-        <v>39583633</v>
+        <v>99999266</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>25BFF91</v>
+        <v>5F5DE22</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="5"/>
@@ -1073,7 +1660,7 @@
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="6"/>
-        <v>39583633</v>
+        <v>99999266</v>
       </c>
     </row>
     <row r="21" spans="8:15">
@@ -1091,11 +1678,11 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="3"/>
-        <v>56406556</v>
+        <v>99999805</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>35CB21C</v>
+        <v>5F5E03D</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="5"/>
@@ -1103,7 +1690,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="6"/>
-        <v>56406556</v>
+        <v>99999805</v>
       </c>
     </row>
     <row r="22" spans="8:15">
@@ -1121,11 +1708,11 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="3"/>
-        <v>36371482</v>
+        <v>99999967</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>22AFC1A</v>
+        <v>5F5E0DF</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="5"/>
@@ -1133,7 +1720,7 @@
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="6"/>
-        <v>36371482</v>
+        <v>99999967</v>
       </c>
     </row>
     <row r="23" spans="8:15">
@@ -1151,11 +1738,11 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="3"/>
-        <v>49025968</v>
+        <v>99999364</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>2EC13B0</v>
+        <v>5F5DE84</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="5"/>
@@ -1163,7 +1750,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="6"/>
-        <v>49025968</v>
+        <v>99999364</v>
       </c>
     </row>
     <row r="24" spans="8:15">
@@ -1181,11 +1768,11 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="3"/>
-        <v>23685000</v>
+        <v>99999231</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1696788</v>
+        <v>5F5DDFF</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="5"/>
@@ -1193,7 +1780,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="6"/>
-        <v>23685000</v>
+        <v>99999231</v>
       </c>
     </row>
     <row r="25" spans="8:15">
@@ -1211,11 +1798,11 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="3"/>
-        <v>95526741</v>
+        <v>99999290</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5B19F55</v>
+        <v>5F5DE3A</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="5"/>
@@ -1223,7 +1810,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="6"/>
-        <v>95526741</v>
+        <v>99999290</v>
       </c>
     </row>
     <row r="26" spans="8:15">
@@ -1241,11 +1828,11 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="3"/>
-        <v>90076717</v>
+        <v>99999633</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>55E762D</v>
+        <v>5F5DF91</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="5"/>
@@ -1253,7 +1840,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="6"/>
-        <v>90076717</v>
+        <v>99999633</v>
       </c>
     </row>
     <row r="27" spans="8:15">
@@ -1271,11 +1858,11 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="3"/>
-        <v>71872649</v>
+        <v>99999246</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>448B089</v>
+        <v>5F5DE0E</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="5"/>
@@ -1283,7 +1870,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="6"/>
-        <v>71872649</v>
+        <v>99999246</v>
       </c>
     </row>
     <row r="28" spans="8:15">
@@ -1301,11 +1888,11 @@
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="3"/>
-        <v>75214625</v>
+        <v>99999863</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>47BAF21</v>
+        <v>5F5E077</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="5"/>
@@ -1313,7 +1900,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="6"/>
-        <v>75214625</v>
+        <v>99999863</v>
       </c>
     </row>
     <row r="29" spans="8:15">
@@ -1331,11 +1918,11 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="3"/>
-        <v>24574446</v>
+        <v>99999906</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>176F9EE</v>
+        <v>5F5E0A2</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="5"/>
@@ -1343,17 +1930,17 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="6"/>
-        <v>24574446</v>
+        <v>99999906</v>
       </c>
     </row>
     <row r="30" spans="8:15">
       <c r="L30">
         <f t="shared" ca="1" si="3"/>
-        <v>77315111</v>
+        <v>99999465</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>49BBC27</v>
+        <v>5F5DEE9</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="5"/>
@@ -1361,17 +1948,17 @@
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="6"/>
-        <v>77315111</v>
+        <v>99999465</v>
       </c>
     </row>
     <row r="31" spans="8:15">
       <c r="L31">
         <f t="shared" ca="1" si="3"/>
-        <v>63434622</v>
+        <v>99999584</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>3C7EF7E</v>
+        <v>5F5DF60</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="5"/>
@@ -1379,17 +1966,17 @@
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="6"/>
-        <v>63434622</v>
+        <v>99999584</v>
       </c>
     </row>
     <row r="32" spans="8:15">
       <c r="L32">
         <f t="shared" ca="1" si="3"/>
-        <v>31716060</v>
+        <v>99999589</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1E3F2DC</v>
+        <v>5F5DF65</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="5"/>
@@ -1397,17 +1984,17 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="6"/>
-        <v>31716060</v>
+        <v>99999589</v>
       </c>
     </row>
     <row r="33" spans="12:15">
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
-        <v>90616689</v>
+        <v>99999733</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>566B371</v>
+        <v>5F5DFF5</v>
       </c>
       <c r="N33">
         <f t="shared" ca="1" si="5"/>
@@ -1415,17 +2002,17 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="6"/>
-        <v>90616689</v>
+        <v>99999733</v>
       </c>
     </row>
     <row r="34" spans="12:15">
       <c r="L34">
         <f t="shared" ca="1" si="3"/>
-        <v>40649957</v>
+        <v>99999824</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>26C44E5</v>
+        <v>5F5E050</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="5"/>
@@ -1433,17 +2020,17 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="6"/>
-        <v>40649957</v>
+        <v>99999824</v>
       </c>
     </row>
     <row r="35" spans="12:15">
       <c r="L35">
         <f t="shared" ca="1" si="3"/>
-        <v>26274462</v>
+        <v>99999634</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>190EA9E</v>
+        <v>5F5DF92</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="5"/>
@@ -1451,17 +2038,17 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="6"/>
-        <v>26274462</v>
+        <v>99999634</v>
       </c>
     </row>
     <row r="36" spans="12:15">
       <c r="L36">
         <f t="shared" ca="1" si="3"/>
-        <v>74508442</v>
+        <v>99999236</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>470E89A</v>
+        <v>5F5DE04</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="5"/>
@@ -1469,17 +2056,17 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="6"/>
-        <v>74508442</v>
+        <v>99999236</v>
       </c>
     </row>
     <row r="37" spans="12:15">
       <c r="L37">
         <f t="shared" ca="1" si="3"/>
-        <v>78134082</v>
+        <v>99999971</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>4A83B42</v>
+        <v>5F5E0E3</v>
       </c>
       <c r="N37">
         <f t="shared" ca="1" si="5"/>
@@ -1487,17 +2074,17 @@
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="6"/>
-        <v>78134082</v>
+        <v>99999971</v>
       </c>
     </row>
     <row r="38" spans="12:15">
       <c r="L38">
         <f t="shared" ca="1" si="3"/>
-        <v>91962055</v>
+        <v>99999071</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>57B3AC7</v>
+        <v>5F5DD5F</v>
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="5"/>
@@ -1505,17 +2092,17 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="6"/>
-        <v>91962055</v>
+        <v>99999071</v>
       </c>
     </row>
     <row r="39" spans="12:15">
       <c r="L39">
         <f t="shared" ca="1" si="3"/>
-        <v>55342651</v>
+        <v>99999849</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>34C763B</v>
+        <v>5F5E069</v>
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="5"/>
@@ -1523,17 +2110,17 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="6"/>
-        <v>55342651</v>
+        <v>99999849</v>
       </c>
     </row>
     <row r="40" spans="12:15">
       <c r="L40">
         <f t="shared" ca="1" si="3"/>
-        <v>29278183</v>
+        <v>99999286</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1BEBFE7</v>
+        <v>5F5DE36</v>
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="5"/>
@@ -1541,184 +2128,11 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="6"/>
-        <v>29278183</v>
+        <v>99999286</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="G4:G71"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="7:7">
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="7:7">
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="7:7">
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="7:7">
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="7:7">
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="7:7">
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="7:7">
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="7:7">
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="7:7">
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="7:7">
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="7:7">
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="7:7">
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="7:7">
-      <c r="G16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7">
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7">
-      <c r="G20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7">
-      <c r="G24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7">
-      <c r="G34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="7:7">
-      <c r="G35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="7:7">
-      <c r="G45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="7:7">
-      <c r="G50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7">
-      <c r="G51" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="7:7">
-      <c r="G52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="7:7">
-      <c r="G53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7">
-      <c r="G54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="7:7">
-      <c r="G55" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="7:7">
-      <c r="G57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="7:7">
-      <c r="G64" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="7:7">
-      <c r="G69" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71" spans="7:7">
-      <c r="G71" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
EA:functions imported to ARCHI!
</commit_message>
<xml_diff>
--- a/import/generator.xlsx
+++ b/import/generator.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Business Processes" sheetId="1" r:id="rId1"/>
-    <sheet name="Applications" sheetId="2" r:id="rId2"/>
-    <sheet name="ID" sheetId="3" r:id="rId3"/>
+    <sheet name="Applications" sheetId="2" r:id="rId1"/>
+    <sheet name="AppFunctions" sheetId="4" r:id="rId2"/>
+    <sheet name="Business Processes" sheetId="1" r:id="rId3"/>
+    <sheet name="ID" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ID!$L$2:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ID!$L$2:$O$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>2c19695</t>
   </si>
@@ -496,6 +497,9 @@
   </si>
   <si>
     <t>predesle kroky</t>
+  </si>
+  <si>
+    <t>Pro kazdy package level 1 vyrobit Aplikacni Funkci a do ni kompozici pridat obsah package.</t>
   </si>
 </sst>
 </file>
@@ -889,6 +893,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -902,157 +1081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:O20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:O40"/>
   <sheetViews>
@@ -1132,11 +1161,11 @@
       </c>
       <c r="L3">
         <f ca="1">RANDBETWEEN($G$4,$G$5)</f>
-        <v>99999996</v>
+        <v>99999119</v>
       </c>
       <c r="M3" t="str">
         <f ca="1">DEC2HEX(L3)</f>
-        <v>5F5E0FC</v>
+        <v>5F5DD8F</v>
       </c>
       <c r="N3">
         <f ca="1">LEN(M3)</f>
@@ -1144,7 +1173,7 @@
       </c>
       <c r="O3">
         <f ca="1">HEX2DEC(M3)</f>
-        <v>99999996</v>
+        <v>99999119</v>
       </c>
     </row>
     <row r="4" spans="2:15">
@@ -1165,11 +1194,11 @@
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L40" ca="1" si="3">RANDBETWEEN($G$4,$G$5)</f>
-        <v>99999970</v>
+        <v>99999097</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M40" ca="1" si="4">DEC2HEX(L4)</f>
-        <v>5F5E0E2</v>
+        <v>5F5DD79</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N40" ca="1" si="5">LEN(M4)</f>
@@ -1177,7 +1206,7 @@
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O40" ca="1" si="6">HEX2DEC(M4)</f>
-        <v>99999970</v>
+        <v>99999097</v>
       </c>
     </row>
     <row r="5" spans="2:15">
@@ -1198,11 +1227,11 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="3"/>
-        <v>99999489</v>
+        <v>99999396</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF01</v>
+        <v>5F5DEA4</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="5"/>
@@ -1210,7 +1239,7 @@
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="6"/>
-        <v>99999489</v>
+        <v>99999396</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1228,11 +1257,11 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="3"/>
-        <v>99999570</v>
+        <v>99999754</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF52</v>
+        <v>5F5E00A</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="5"/>
@@ -1240,7 +1269,7 @@
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="6"/>
-        <v>99999570</v>
+        <v>99999754</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -1258,11 +1287,11 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="3"/>
-        <v>99999004</v>
+        <v>99999706</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD1C</v>
+        <v>5F5DFDA</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="5"/>
@@ -1270,7 +1299,7 @@
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="6"/>
-        <v>99999004</v>
+        <v>99999706</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -1288,11 +1317,11 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="3"/>
-        <v>99999546</v>
+        <v>99999024</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF3A</v>
+        <v>5F5DD30</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="5"/>
@@ -1300,7 +1329,7 @@
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="6"/>
-        <v>99999546</v>
+        <v>99999024</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -1318,11 +1347,11 @@
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="3"/>
-        <v>99999930</v>
+        <v>99999713</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0BA</v>
+        <v>5F5DFE1</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="5"/>
@@ -1330,7 +1359,7 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="6"/>
-        <v>99999930</v>
+        <v>99999713</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -1348,11 +1377,11 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="3"/>
-        <v>99999407</v>
+        <v>99999357</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEAF</v>
+        <v>5F5DE7D</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="5"/>
@@ -1360,7 +1389,7 @@
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="6"/>
-        <v>99999407</v>
+        <v>99999357</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -1378,11 +1407,11 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="3"/>
-        <v>99999149</v>
+        <v>99999266</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDAD</v>
+        <v>5F5DE22</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="5"/>
@@ -1390,7 +1419,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="6"/>
-        <v>99999149</v>
+        <v>99999266</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -1408,11 +1437,11 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="3"/>
-        <v>99999758</v>
+        <v>99999944</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E00E</v>
+        <v>5F5E0C8</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="5"/>
@@ -1420,7 +1449,7 @@
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="6"/>
-        <v>99999758</v>
+        <v>99999944</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -1438,11 +1467,11 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>99999390</v>
+        <v>99999560</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE9E</v>
+        <v>5F5DF48</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="5"/>
@@ -1450,7 +1479,7 @@
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="6"/>
-        <v>99999390</v>
+        <v>99999560</v>
       </c>
     </row>
     <row r="14" spans="2:15">
@@ -1468,11 +1497,11 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>99999460</v>
+        <v>99999101</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEE4</v>
+        <v>5F5DD7D</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="5"/>
@@ -1480,7 +1509,7 @@
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="6"/>
-        <v>99999460</v>
+        <v>99999101</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -1498,11 +1527,11 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>99999050</v>
+        <v>99999646</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD4A</v>
+        <v>5F5DF9E</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="5"/>
@@ -1510,7 +1539,7 @@
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="6"/>
-        <v>99999050</v>
+        <v>99999646</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -1528,11 +1557,11 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
-        <v>99999668</v>
+        <v>99999318</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFB4</v>
+        <v>5F5DE56</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="5"/>
@@ -1540,7 +1569,7 @@
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="6"/>
-        <v>99999668</v>
+        <v>99999318</v>
       </c>
     </row>
     <row r="17" spans="8:15">
@@ -1558,11 +1587,11 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>99999803</v>
+        <v>99999464</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E03B</v>
+        <v>5F5DEE8</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="5"/>
@@ -1570,7 +1599,7 @@
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="6"/>
-        <v>99999803</v>
+        <v>99999464</v>
       </c>
     </row>
     <row r="18" spans="8:15">
@@ -1588,11 +1617,11 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="3"/>
-        <v>99999289</v>
+        <v>99999865</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE39</v>
+        <v>5F5E079</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="5"/>
@@ -1600,7 +1629,7 @@
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="6"/>
-        <v>99999289</v>
+        <v>99999865</v>
       </c>
     </row>
     <row r="19" spans="8:15">
@@ -1618,11 +1647,11 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>99999024</v>
+        <v>99999170</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD30</v>
+        <v>5F5DDC2</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="5"/>
@@ -1630,7 +1659,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="6"/>
-        <v>99999024</v>
+        <v>99999170</v>
       </c>
     </row>
     <row r="20" spans="8:15">
@@ -1648,11 +1677,11 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="3"/>
-        <v>99999266</v>
+        <v>99999148</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE22</v>
+        <v>5F5DDAC</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="5"/>
@@ -1660,7 +1689,7 @@
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="6"/>
-        <v>99999266</v>
+        <v>99999148</v>
       </c>
     </row>
     <row r="21" spans="8:15">
@@ -1678,11 +1707,11 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="3"/>
-        <v>99999805</v>
+        <v>99999248</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E03D</v>
+        <v>5F5DE10</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="5"/>
@@ -1690,7 +1719,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="6"/>
-        <v>99999805</v>
+        <v>99999248</v>
       </c>
     </row>
     <row r="22" spans="8:15">
@@ -1708,11 +1737,11 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="3"/>
-        <v>99999967</v>
+        <v>99999298</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0DF</v>
+        <v>5F5DE42</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="5"/>
@@ -1720,7 +1749,7 @@
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="6"/>
-        <v>99999967</v>
+        <v>99999298</v>
       </c>
     </row>
     <row r="23" spans="8:15">
@@ -1738,11 +1767,11 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="3"/>
-        <v>99999364</v>
+        <v>99999299</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE84</v>
+        <v>5F5DE43</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="5"/>
@@ -1750,7 +1779,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="6"/>
-        <v>99999364</v>
+        <v>99999299</v>
       </c>
     </row>
     <row r="24" spans="8:15">
@@ -1768,11 +1797,11 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="3"/>
-        <v>99999231</v>
+        <v>99999828</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDFF</v>
+        <v>5F5E054</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="5"/>
@@ -1780,7 +1809,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="6"/>
-        <v>99999231</v>
+        <v>99999828</v>
       </c>
     </row>
     <row r="25" spans="8:15">
@@ -1798,11 +1827,11 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="3"/>
-        <v>99999290</v>
+        <v>99999295</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE3A</v>
+        <v>5F5DE3F</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="5"/>
@@ -1810,7 +1839,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="6"/>
-        <v>99999290</v>
+        <v>99999295</v>
       </c>
     </row>
     <row r="26" spans="8:15">
@@ -1828,11 +1857,11 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="3"/>
-        <v>99999633</v>
+        <v>99999536</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF91</v>
+        <v>5F5DF30</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="5"/>
@@ -1840,7 +1869,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="6"/>
-        <v>99999633</v>
+        <v>99999536</v>
       </c>
     </row>
     <row r="27" spans="8:15">
@@ -1858,11 +1887,11 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="3"/>
-        <v>99999246</v>
+        <v>99999257</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE0E</v>
+        <v>5F5DE19</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="5"/>
@@ -1870,7 +1899,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="6"/>
-        <v>99999246</v>
+        <v>99999257</v>
       </c>
     </row>
     <row r="28" spans="8:15">
@@ -1888,11 +1917,11 @@
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="3"/>
-        <v>99999863</v>
+        <v>99999492</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E077</v>
+        <v>5F5DF04</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="5"/>
@@ -1900,7 +1929,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="6"/>
-        <v>99999863</v>
+        <v>99999492</v>
       </c>
     </row>
     <row r="29" spans="8:15">
@@ -1918,11 +1947,11 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="3"/>
-        <v>99999906</v>
+        <v>99999357</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0A2</v>
+        <v>5F5DE7D</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="5"/>
@@ -1930,17 +1959,17 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="6"/>
-        <v>99999906</v>
+        <v>99999357</v>
       </c>
     </row>
     <row r="30" spans="8:15">
       <c r="L30">
         <f t="shared" ca="1" si="3"/>
-        <v>99999465</v>
+        <v>99999244</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEE9</v>
+        <v>5F5DE0C</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="5"/>
@@ -1948,17 +1977,17 @@
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="6"/>
-        <v>99999465</v>
+        <v>99999244</v>
       </c>
     </row>
     <row r="31" spans="8:15">
       <c r="L31">
         <f t="shared" ca="1" si="3"/>
-        <v>99999584</v>
+        <v>99999654</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF60</v>
+        <v>5F5DFA6</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="5"/>
@@ -1966,17 +1995,17 @@
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="6"/>
-        <v>99999584</v>
+        <v>99999654</v>
       </c>
     </row>
     <row r="32" spans="8:15">
       <c r="L32">
         <f t="shared" ca="1" si="3"/>
-        <v>99999589</v>
+        <v>99999690</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF65</v>
+        <v>5F5DFCA</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="5"/>
@@ -1984,17 +2013,17 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="6"/>
-        <v>99999589</v>
+        <v>99999690</v>
       </c>
     </row>
     <row r="33" spans="12:15">
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
-        <v>99999733</v>
+        <v>99999094</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFF5</v>
+        <v>5F5DD76</v>
       </c>
       <c r="N33">
         <f t="shared" ca="1" si="5"/>
@@ -2002,17 +2031,17 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="6"/>
-        <v>99999733</v>
+        <v>99999094</v>
       </c>
     </row>
     <row r="34" spans="12:15">
       <c r="L34">
         <f t="shared" ca="1" si="3"/>
-        <v>99999824</v>
+        <v>99999242</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E050</v>
+        <v>5F5DE0A</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="5"/>
@@ -2020,17 +2049,17 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="6"/>
-        <v>99999824</v>
+        <v>99999242</v>
       </c>
     </row>
     <row r="35" spans="12:15">
       <c r="L35">
         <f t="shared" ca="1" si="3"/>
-        <v>99999634</v>
+        <v>99999962</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF92</v>
+        <v>5F5E0DA</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="5"/>
@@ -2038,17 +2067,17 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="6"/>
-        <v>99999634</v>
+        <v>99999962</v>
       </c>
     </row>
     <row r="36" spans="12:15">
       <c r="L36">
         <f t="shared" ca="1" si="3"/>
-        <v>99999236</v>
+        <v>99999875</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE04</v>
+        <v>5F5E083</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="5"/>
@@ -2056,17 +2085,17 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="6"/>
-        <v>99999236</v>
+        <v>99999875</v>
       </c>
     </row>
     <row r="37" spans="12:15">
       <c r="L37">
         <f t="shared" ca="1" si="3"/>
-        <v>99999971</v>
+        <v>99999111</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0E3</v>
+        <v>5F5DD87</v>
       </c>
       <c r="N37">
         <f t="shared" ca="1" si="5"/>
@@ -2074,17 +2103,17 @@
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="6"/>
-        <v>99999971</v>
+        <v>99999111</v>
       </c>
     </row>
     <row r="38" spans="12:15">
       <c r="L38">
         <f t="shared" ca="1" si="3"/>
-        <v>99999071</v>
+        <v>99999186</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD5F</v>
+        <v>5F5DDD2</v>
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="5"/>
@@ -2092,17 +2121,17 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="6"/>
-        <v>99999071</v>
+        <v>99999186</v>
       </c>
     </row>
     <row r="39" spans="12:15">
       <c r="L39">
         <f t="shared" ca="1" si="3"/>
-        <v>99999849</v>
+        <v>99999497</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E069</v>
+        <v>5F5DF09</v>
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="5"/>
@@ -2110,17 +2139,17 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="6"/>
-        <v>99999849</v>
+        <v>99999497</v>
       </c>
     </row>
     <row r="40" spans="12:15">
       <c r="L40">
         <f t="shared" ca="1" si="3"/>
-        <v>99999286</v>
+        <v>99999199</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE36</v>
+        <v>5F5DDDF</v>
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="5"/>
@@ -2128,7 +2157,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="6"/>
-        <v>99999286</v>
+        <v>99999199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EA:processess imported to ARCHI!
</commit_message>
<xml_diff>
--- a/import/generator.xlsx
+++ b/import/generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Applications" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>2c19695</t>
   </si>
@@ -500,6 +500,139 @@
   </si>
   <si>
     <t>Pro kazdy package level 1 vyrobit Aplikacni Funkci a do ni kompozici pridat obsah package.</t>
+  </si>
+  <si>
+    <t>Jedu pres packages strukturu;  &lt;packagedElement xmi:type="uml:Package" tvori hierarchizaci procesu.</t>
+  </si>
+  <si>
+    <t>V ramci neho muzou byt POOLS &lt;group xmi:type="uml:ActivityPartition" x jako Aktor   a v nem dalsi activity ci pools &lt;node xmi:idref="EAID…</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>pro element idrefu hledam v extensions element daneho ide refu a v nem podrizeny element properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client's data are taken from </t>
+  </si>
+  <si>
+    <t>86DDF151-5541-411a-B373-F2629715741C</t>
+  </si>
+  <si>
+    <t>nerealiz</t>
+  </si>
+  <si>
+    <t>Prvni aktivity &lt;packagedElement xmi:type="uml:Activity"   je realny BP. Activities v ramci nej jsou jednotlive kroky procesu. Staci 1 level. Tento level oznacim v nazvu prefixem activity. Pro jistotu. Jinak pouzivam vsude Composition.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;element xsi:type="archimate:BusinessProcess" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>26dc16a5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Nadr"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;element xsi:type="archimate:BusinessProcess" id="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0f06008f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" name="Podr"/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;element xsi:type="archimate:CompositionRelationship" id="1408e2fa" source="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>26dc16a5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" target="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0f06008f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"/&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -895,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -1068,14 +1201,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:17">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="Q14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="Q15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1161,11 +1357,11 @@
       </c>
       <c r="L3">
         <f ca="1">RANDBETWEEN($G$4,$G$5)</f>
-        <v>99999119</v>
+        <v>99999327</v>
       </c>
       <c r="M3" t="str">
         <f ca="1">DEC2HEX(L3)</f>
-        <v>5F5DD8F</v>
+        <v>5F5DE5F</v>
       </c>
       <c r="N3">
         <f ca="1">LEN(M3)</f>
@@ -1173,7 +1369,7 @@
       </c>
       <c r="O3">
         <f ca="1">HEX2DEC(M3)</f>
-        <v>99999119</v>
+        <v>99999327</v>
       </c>
     </row>
     <row r="4" spans="2:15">
@@ -1194,11 +1390,11 @@
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L40" ca="1" si="3">RANDBETWEEN($G$4,$G$5)</f>
-        <v>99999097</v>
+        <v>99999118</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M40" ca="1" si="4">DEC2HEX(L4)</f>
-        <v>5F5DD79</v>
+        <v>5F5DD8E</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N40" ca="1" si="5">LEN(M4)</f>
@@ -1206,7 +1402,7 @@
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O40" ca="1" si="6">HEX2DEC(M4)</f>
-        <v>99999097</v>
+        <v>99999118</v>
       </c>
     </row>
     <row r="5" spans="2:15">
@@ -1227,11 +1423,11 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="3"/>
-        <v>99999396</v>
+        <v>99999695</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEA4</v>
+        <v>5F5DFCF</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="5"/>
@@ -1239,7 +1435,7 @@
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="6"/>
-        <v>99999396</v>
+        <v>99999695</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1257,11 +1453,11 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="3"/>
-        <v>99999754</v>
+        <v>99999406</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E00A</v>
+        <v>5F5DEAE</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="5"/>
@@ -1269,7 +1465,7 @@
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="6"/>
-        <v>99999754</v>
+        <v>99999406</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -1287,11 +1483,11 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="3"/>
-        <v>99999706</v>
+        <v>99999732</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFDA</v>
+        <v>5F5DFF4</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="5"/>
@@ -1299,7 +1495,7 @@
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="6"/>
-        <v>99999706</v>
+        <v>99999732</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -1317,11 +1513,11 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="3"/>
-        <v>99999024</v>
+        <v>99999753</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD30</v>
+        <v>5F5E009</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="5"/>
@@ -1329,7 +1525,7 @@
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="6"/>
-        <v>99999024</v>
+        <v>99999753</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -1347,11 +1543,11 @@
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="3"/>
-        <v>99999713</v>
+        <v>99999306</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFE1</v>
+        <v>5F5DE4A</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="5"/>
@@ -1359,7 +1555,7 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="6"/>
-        <v>99999713</v>
+        <v>99999306</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -1377,11 +1573,11 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="3"/>
-        <v>99999357</v>
+        <v>99999396</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE7D</v>
+        <v>5F5DEA4</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="5"/>
@@ -1389,7 +1585,7 @@
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="6"/>
-        <v>99999357</v>
+        <v>99999396</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -1407,11 +1603,11 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="3"/>
-        <v>99999266</v>
+        <v>99999015</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE22</v>
+        <v>5F5DD27</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="5"/>
@@ -1419,7 +1615,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="6"/>
-        <v>99999266</v>
+        <v>99999015</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -1437,11 +1633,11 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="3"/>
-        <v>99999944</v>
+        <v>99999088</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0C8</v>
+        <v>5F5DD70</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="5"/>
@@ -1449,7 +1645,7 @@
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="6"/>
-        <v>99999944</v>
+        <v>99999088</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -1467,11 +1663,11 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>99999560</v>
+        <v>99999507</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF48</v>
+        <v>5F5DF13</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="5"/>
@@ -1479,7 +1675,7 @@
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="6"/>
-        <v>99999560</v>
+        <v>99999507</v>
       </c>
     </row>
     <row r="14" spans="2:15">
@@ -1497,11 +1693,11 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>99999101</v>
+        <v>99999950</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD7D</v>
+        <v>5F5E0CE</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="5"/>
@@ -1509,7 +1705,7 @@
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="6"/>
-        <v>99999101</v>
+        <v>99999950</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -1527,11 +1723,11 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>99999646</v>
+        <v>99999808</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF9E</v>
+        <v>5F5E040</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="5"/>
@@ -1539,7 +1735,7 @@
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="6"/>
-        <v>99999646</v>
+        <v>99999808</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -1557,11 +1753,11 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
-        <v>99999318</v>
+        <v>99999366</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE56</v>
+        <v>5F5DE86</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="5"/>
@@ -1569,7 +1765,7 @@
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="6"/>
-        <v>99999318</v>
+        <v>99999366</v>
       </c>
     </row>
     <row r="17" spans="8:15">
@@ -1587,11 +1783,11 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>99999464</v>
+        <v>99999639</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEE8</v>
+        <v>5F5DF97</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="5"/>
@@ -1599,7 +1795,7 @@
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="6"/>
-        <v>99999464</v>
+        <v>99999639</v>
       </c>
     </row>
     <row r="18" spans="8:15">
@@ -1617,11 +1813,11 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="3"/>
-        <v>99999865</v>
+        <v>99999324</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E079</v>
+        <v>5F5DE5C</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="5"/>
@@ -1629,7 +1825,7 @@
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="6"/>
-        <v>99999865</v>
+        <v>99999324</v>
       </c>
     </row>
     <row r="19" spans="8:15">
@@ -1647,11 +1843,11 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>99999170</v>
+        <v>99999102</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDC2</v>
+        <v>5F5DD7E</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="5"/>
@@ -1659,7 +1855,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="6"/>
-        <v>99999170</v>
+        <v>99999102</v>
       </c>
     </row>
     <row r="20" spans="8:15">
@@ -1677,11 +1873,11 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="3"/>
-        <v>99999148</v>
+        <v>99999300</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDAC</v>
+        <v>5F5DE44</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="5"/>
@@ -1689,7 +1885,7 @@
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="6"/>
-        <v>99999148</v>
+        <v>99999300</v>
       </c>
     </row>
     <row r="21" spans="8:15">
@@ -1707,11 +1903,11 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="3"/>
-        <v>99999248</v>
+        <v>99999882</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE10</v>
+        <v>5F5E08A</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="5"/>
@@ -1719,7 +1915,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="6"/>
-        <v>99999248</v>
+        <v>99999882</v>
       </c>
     </row>
     <row r="22" spans="8:15">
@@ -1737,11 +1933,11 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="3"/>
-        <v>99999298</v>
+        <v>99999477</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE42</v>
+        <v>5F5DEF5</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="5"/>
@@ -1749,7 +1945,7 @@
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="6"/>
-        <v>99999298</v>
+        <v>99999477</v>
       </c>
     </row>
     <row r="23" spans="8:15">
@@ -1767,11 +1963,11 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="3"/>
-        <v>99999299</v>
+        <v>99999353</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE43</v>
+        <v>5F5DE79</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="5"/>
@@ -1779,7 +1975,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="6"/>
-        <v>99999299</v>
+        <v>99999353</v>
       </c>
     </row>
     <row r="24" spans="8:15">
@@ -1797,11 +1993,11 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="3"/>
-        <v>99999828</v>
+        <v>99999675</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E054</v>
+        <v>5F5DFBB</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="5"/>
@@ -1809,7 +2005,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="6"/>
-        <v>99999828</v>
+        <v>99999675</v>
       </c>
     </row>
     <row r="25" spans="8:15">
@@ -1827,11 +2023,11 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="3"/>
-        <v>99999295</v>
+        <v>99999098</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE3F</v>
+        <v>5F5DD7A</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="5"/>
@@ -1839,7 +2035,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="6"/>
-        <v>99999295</v>
+        <v>99999098</v>
       </c>
     </row>
     <row r="26" spans="8:15">
@@ -1857,11 +2053,11 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="3"/>
-        <v>99999536</v>
+        <v>99999624</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF30</v>
+        <v>5F5DF88</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="5"/>
@@ -1869,7 +2065,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="6"/>
-        <v>99999536</v>
+        <v>99999624</v>
       </c>
     </row>
     <row r="27" spans="8:15">
@@ -1887,11 +2083,11 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="3"/>
-        <v>99999257</v>
+        <v>99999055</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE19</v>
+        <v>5F5DD4F</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="5"/>
@@ -1899,7 +2095,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="6"/>
-        <v>99999257</v>
+        <v>99999055</v>
       </c>
     </row>
     <row r="28" spans="8:15">
@@ -1917,11 +2113,11 @@
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="3"/>
-        <v>99999492</v>
+        <v>99999071</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF04</v>
+        <v>5F5DD5F</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="5"/>
@@ -1929,7 +2125,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="6"/>
-        <v>99999492</v>
+        <v>99999071</v>
       </c>
     </row>
     <row r="29" spans="8:15">
@@ -1947,11 +2143,11 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="3"/>
-        <v>99999357</v>
+        <v>99999784</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE7D</v>
+        <v>5F5E028</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="5"/>
@@ -1959,17 +2155,17 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="6"/>
-        <v>99999357</v>
+        <v>99999784</v>
       </c>
     </row>
     <row r="30" spans="8:15">
       <c r="L30">
         <f t="shared" ca="1" si="3"/>
-        <v>99999244</v>
+        <v>99999243</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE0C</v>
+        <v>5F5DE0B</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="5"/>
@@ -1977,17 +2173,17 @@
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="6"/>
-        <v>99999244</v>
+        <v>99999243</v>
       </c>
     </row>
     <row r="31" spans="8:15">
       <c r="L31">
         <f t="shared" ca="1" si="3"/>
-        <v>99999654</v>
+        <v>99999494</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFA6</v>
+        <v>5F5DF06</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="5"/>
@@ -1995,17 +2191,17 @@
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="6"/>
-        <v>99999654</v>
+        <v>99999494</v>
       </c>
     </row>
     <row r="32" spans="8:15">
       <c r="L32">
         <f t="shared" ca="1" si="3"/>
-        <v>99999690</v>
+        <v>99999647</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFCA</v>
+        <v>5F5DF9F</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="5"/>
@@ -2013,17 +2209,17 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="6"/>
-        <v>99999690</v>
+        <v>99999647</v>
       </c>
     </row>
     <row r="33" spans="12:15">
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
-        <v>99999094</v>
+        <v>99999210</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD76</v>
+        <v>5F5DDEA</v>
       </c>
       <c r="N33">
         <f t="shared" ca="1" si="5"/>
@@ -2031,17 +2227,17 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="6"/>
-        <v>99999094</v>
+        <v>99999210</v>
       </c>
     </row>
     <row r="34" spans="12:15">
       <c r="L34">
         <f t="shared" ca="1" si="3"/>
-        <v>99999242</v>
+        <v>99999151</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE0A</v>
+        <v>5F5DDAF</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="5"/>
@@ -2049,17 +2245,17 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="6"/>
-        <v>99999242</v>
+        <v>99999151</v>
       </c>
     </row>
     <row r="35" spans="12:15">
       <c r="L35">
         <f t="shared" ca="1" si="3"/>
-        <v>99999962</v>
+        <v>99999227</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0DA</v>
+        <v>5F5DDFB</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="5"/>
@@ -2067,17 +2263,17 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="6"/>
-        <v>99999962</v>
+        <v>99999227</v>
       </c>
     </row>
     <row r="36" spans="12:15">
       <c r="L36">
         <f t="shared" ca="1" si="3"/>
-        <v>99999875</v>
+        <v>99999990</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E083</v>
+        <v>5F5E0F6</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="5"/>
@@ -2085,17 +2281,17 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="6"/>
-        <v>99999875</v>
+        <v>99999990</v>
       </c>
     </row>
     <row r="37" spans="12:15">
       <c r="L37">
         <f t="shared" ca="1" si="3"/>
-        <v>99999111</v>
+        <v>99999504</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD87</v>
+        <v>5F5DF10</v>
       </c>
       <c r="N37">
         <f t="shared" ca="1" si="5"/>
@@ -2103,17 +2299,17 @@
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="6"/>
-        <v>99999111</v>
+        <v>99999504</v>
       </c>
     </row>
     <row r="38" spans="12:15">
       <c r="L38">
         <f t="shared" ca="1" si="3"/>
-        <v>99999186</v>
+        <v>99999780</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDD2</v>
+        <v>5F5E024</v>
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="5"/>
@@ -2121,17 +2317,17 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="6"/>
-        <v>99999186</v>
+        <v>99999780</v>
       </c>
     </row>
     <row r="39" spans="12:15">
       <c r="L39">
         <f t="shared" ca="1" si="3"/>
-        <v>99999497</v>
+        <v>99999334</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF09</v>
+        <v>5F5DE66</v>
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="5"/>
@@ -2139,17 +2335,17 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="6"/>
-        <v>99999497</v>
+        <v>99999334</v>
       </c>
     </row>
     <row r="40" spans="12:15">
       <c r="L40">
         <f t="shared" ca="1" si="3"/>
-        <v>99999199</v>
+        <v>99999818</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDDF</v>
+        <v>5F5E04A</v>
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="5"/>
@@ -2157,7 +2353,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="6"/>
-        <v>99999199</v>
+        <v>99999818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Archi: BSL conected to the functions. ARCHI model internal batch processing
</commit_message>
<xml_diff>
--- a/import/generator.xlsx
+++ b/import/generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Applications" sheetId="2" r:id="rId1"/>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1203,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1357,11 +1357,11 @@
       </c>
       <c r="L3">
         <f ca="1">RANDBETWEEN($G$4,$G$5)</f>
-        <v>99999327</v>
+        <v>99999314</v>
       </c>
       <c r="M3" t="str">
         <f ca="1">DEC2HEX(L3)</f>
-        <v>5F5DE5F</v>
+        <v>5F5DE52</v>
       </c>
       <c r="N3">
         <f ca="1">LEN(M3)</f>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="O3">
         <f ca="1">HEX2DEC(M3)</f>
-        <v>99999327</v>
+        <v>99999314</v>
       </c>
     </row>
     <row r="4" spans="2:15">
@@ -1390,11 +1390,11 @@
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L40" ca="1" si="3">RANDBETWEEN($G$4,$G$5)</f>
-        <v>99999118</v>
+        <v>99999165</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M40" ca="1" si="4">DEC2HEX(L4)</f>
-        <v>5F5DD8E</v>
+        <v>5F5DDBD</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N40" ca="1" si="5">LEN(M4)</f>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O40" ca="1" si="6">HEX2DEC(M4)</f>
-        <v>99999118</v>
+        <v>99999165</v>
       </c>
     </row>
     <row r="5" spans="2:15">
@@ -1423,11 +1423,11 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="3"/>
-        <v>99999695</v>
+        <v>99999806</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFCF</v>
+        <v>5F5E03E</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="5"/>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="6"/>
-        <v>99999695</v>
+        <v>99999806</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1453,11 +1453,11 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="3"/>
-        <v>99999406</v>
+        <v>99999128</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEAE</v>
+        <v>5F5DD98</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="5"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="6"/>
-        <v>99999406</v>
+        <v>99999128</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -1483,11 +1483,11 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="3"/>
-        <v>99999732</v>
+        <v>99999579</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFF4</v>
+        <v>5F5DF5B</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="5"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="6"/>
-        <v>99999732</v>
+        <v>99999579</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -1513,11 +1513,11 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="3"/>
-        <v>99999753</v>
+        <v>99999909</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E009</v>
+        <v>5F5E0A5</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="5"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="6"/>
-        <v>99999753</v>
+        <v>99999909</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="3"/>
-        <v>99999306</v>
+        <v>99999509</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE4A</v>
+        <v>5F5DF15</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="5"/>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="6"/>
-        <v>99999306</v>
+        <v>99999509</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -1573,11 +1573,11 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="3"/>
-        <v>99999396</v>
+        <v>99999923</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEA4</v>
+        <v>5F5E0B3</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="5"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="6"/>
-        <v>99999396</v>
+        <v>99999923</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -1603,11 +1603,11 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="3"/>
-        <v>99999015</v>
+        <v>99999378</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD27</v>
+        <v>5F5DE92</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="5"/>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="6"/>
-        <v>99999015</v>
+        <v>99999378</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -1633,11 +1633,11 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="3"/>
-        <v>99999088</v>
+        <v>99999671</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD70</v>
+        <v>5F5DFB7</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="5"/>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="6"/>
-        <v>99999088</v>
+        <v>99999671</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -1663,11 +1663,11 @@
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="3"/>
-        <v>99999507</v>
+        <v>99999162</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF13</v>
+        <v>5F5DDBA</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="5"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="6"/>
-        <v>99999507</v>
+        <v>99999162</v>
       </c>
     </row>
     <row r="14" spans="2:15">
@@ -1693,11 +1693,11 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>99999950</v>
+        <v>99999877</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0CE</v>
+        <v>5F5E085</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="5"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="6"/>
-        <v>99999950</v>
+        <v>99999877</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -1723,11 +1723,11 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>99999808</v>
+        <v>99999940</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E040</v>
+        <v>5F5E0C4</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="5"/>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="6"/>
-        <v>99999808</v>
+        <v>99999940</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -1753,11 +1753,11 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
-        <v>99999366</v>
+        <v>99999781</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE86</v>
+        <v>5F5E025</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="5"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="6"/>
-        <v>99999366</v>
+        <v>99999781</v>
       </c>
     </row>
     <row r="17" spans="8:15">
@@ -1783,11 +1783,11 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>99999639</v>
+        <v>99999899</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF97</v>
+        <v>5F5E09B</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="5"/>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="6"/>
-        <v>99999639</v>
+        <v>99999899</v>
       </c>
     </row>
     <row r="18" spans="8:15">
@@ -1813,11 +1813,11 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="3"/>
-        <v>99999324</v>
+        <v>99999710</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE5C</v>
+        <v>5F5DFDE</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="5"/>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="6"/>
-        <v>99999324</v>
+        <v>99999710</v>
       </c>
     </row>
     <row r="19" spans="8:15">
@@ -1843,11 +1843,11 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>99999102</v>
+        <v>99999409</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD7E</v>
+        <v>5F5DEB1</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="5"/>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="6"/>
-        <v>99999102</v>
+        <v>99999409</v>
       </c>
     </row>
     <row r="20" spans="8:15">
@@ -1873,11 +1873,11 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="3"/>
-        <v>99999300</v>
+        <v>99999853</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE44</v>
+        <v>5F5E06D</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="5"/>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="6"/>
-        <v>99999300</v>
+        <v>99999853</v>
       </c>
     </row>
     <row r="21" spans="8:15">
@@ -1903,11 +1903,11 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="3"/>
-        <v>99999882</v>
+        <v>99999662</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E08A</v>
+        <v>5F5DFAE</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="5"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="6"/>
-        <v>99999882</v>
+        <v>99999662</v>
       </c>
     </row>
     <row r="22" spans="8:15">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="3"/>
-        <v>99999477</v>
+        <v>99999184</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DEF5</v>
+        <v>5F5DDD0</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="5"/>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="6"/>
-        <v>99999477</v>
+        <v>99999184</v>
       </c>
     </row>
     <row r="23" spans="8:15">
@@ -1963,11 +1963,11 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="3"/>
-        <v>99999353</v>
+        <v>99999786</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE79</v>
+        <v>5F5E02A</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="5"/>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="6"/>
-        <v>99999353</v>
+        <v>99999786</v>
       </c>
     </row>
     <row r="24" spans="8:15">
@@ -1993,11 +1993,11 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="3"/>
-        <v>99999675</v>
+        <v>99999668</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DFBB</v>
+        <v>5F5DFB4</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="5"/>
@@ -2005,7 +2005,7 @@
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="6"/>
-        <v>99999675</v>
+        <v>99999668</v>
       </c>
     </row>
     <row r="25" spans="8:15">
@@ -2023,11 +2023,11 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="3"/>
-        <v>99999098</v>
+        <v>99999373</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD7A</v>
+        <v>5F5DE8D</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="5"/>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="6"/>
-        <v>99999098</v>
+        <v>99999373</v>
       </c>
     </row>
     <row r="26" spans="8:15">
@@ -2053,11 +2053,11 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="3"/>
-        <v>99999624</v>
+        <v>99999806</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF88</v>
+        <v>5F5E03E</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="5"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="6"/>
-        <v>99999624</v>
+        <v>99999806</v>
       </c>
     </row>
     <row r="27" spans="8:15">
@@ -2083,11 +2083,11 @@
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="3"/>
-        <v>99999055</v>
+        <v>99999103</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD4F</v>
+        <v>5F5DD7F</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="5"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="6"/>
-        <v>99999055</v>
+        <v>99999103</v>
       </c>
     </row>
     <row r="28" spans="8:15">
@@ -2113,11 +2113,11 @@
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="3"/>
-        <v>99999071</v>
+        <v>99999721</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DD5F</v>
+        <v>5F5DFE9</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="5"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="6"/>
-        <v>99999071</v>
+        <v>99999721</v>
       </c>
     </row>
     <row r="29" spans="8:15">
@@ -2143,11 +2143,11 @@
       </c>
       <c r="L29">
         <f t="shared" ca="1" si="3"/>
-        <v>99999784</v>
+        <v>99999866</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E028</v>
+        <v>5F5E07A</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="5"/>
@@ -2155,17 +2155,17 @@
       </c>
       <c r="O29">
         <f t="shared" ca="1" si="6"/>
-        <v>99999784</v>
+        <v>99999866</v>
       </c>
     </row>
     <row r="30" spans="8:15">
       <c r="L30">
         <f t="shared" ca="1" si="3"/>
-        <v>99999243</v>
+        <v>99999777</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE0B</v>
+        <v>5F5E021</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="5"/>
@@ -2173,17 +2173,17 @@
       </c>
       <c r="O30">
         <f t="shared" ca="1" si="6"/>
-        <v>99999243</v>
+        <v>99999777</v>
       </c>
     </row>
     <row r="31" spans="8:15">
       <c r="L31">
         <f t="shared" ca="1" si="3"/>
-        <v>99999494</v>
+        <v>99999736</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF06</v>
+        <v>5F5DFF8</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="5"/>
@@ -2191,17 +2191,17 @@
       </c>
       <c r="O31">
         <f t="shared" ca="1" si="6"/>
-        <v>99999494</v>
+        <v>99999736</v>
       </c>
     </row>
     <row r="32" spans="8:15">
       <c r="L32">
         <f t="shared" ca="1" si="3"/>
-        <v>99999647</v>
+        <v>99999903</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF9F</v>
+        <v>5F5E09F</v>
       </c>
       <c r="N32">
         <f t="shared" ca="1" si="5"/>
@@ -2209,17 +2209,17 @@
       </c>
       <c r="O32">
         <f t="shared" ca="1" si="6"/>
-        <v>99999647</v>
+        <v>99999903</v>
       </c>
     </row>
     <row r="33" spans="12:15">
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
-        <v>99999210</v>
+        <v>99999818</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDEA</v>
+        <v>5F5E04A</v>
       </c>
       <c r="N33">
         <f t="shared" ca="1" si="5"/>
@@ -2227,17 +2227,17 @@
       </c>
       <c r="O33">
         <f t="shared" ca="1" si="6"/>
-        <v>99999210</v>
+        <v>99999818</v>
       </c>
     </row>
     <row r="34" spans="12:15">
       <c r="L34">
         <f t="shared" ca="1" si="3"/>
-        <v>99999151</v>
+        <v>99999006</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDAF</v>
+        <v>5F5DD1E</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="5"/>
@@ -2245,17 +2245,17 @@
       </c>
       <c r="O34">
         <f t="shared" ca="1" si="6"/>
-        <v>99999151</v>
+        <v>99999006</v>
       </c>
     </row>
     <row r="35" spans="12:15">
       <c r="L35">
         <f t="shared" ca="1" si="3"/>
-        <v>99999227</v>
+        <v>99999995</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DDFB</v>
+        <v>5F5E0FB</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="5"/>
@@ -2263,17 +2263,17 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="6"/>
-        <v>99999227</v>
+        <v>99999995</v>
       </c>
     </row>
     <row r="36" spans="12:15">
       <c r="L36">
         <f t="shared" ca="1" si="3"/>
-        <v>99999990</v>
+        <v>99999869</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E0F6</v>
+        <v>5F5E07D</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="5"/>
@@ -2281,17 +2281,17 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="6"/>
-        <v>99999990</v>
+        <v>99999869</v>
       </c>
     </row>
     <row r="37" spans="12:15">
       <c r="L37">
         <f t="shared" ca="1" si="3"/>
-        <v>99999504</v>
+        <v>99999004</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DF10</v>
+        <v>5F5DD1C</v>
       </c>
       <c r="N37">
         <f t="shared" ca="1" si="5"/>
@@ -2299,17 +2299,17 @@
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="6"/>
-        <v>99999504</v>
+        <v>99999004</v>
       </c>
     </row>
     <row r="38" spans="12:15">
       <c r="L38">
         <f t="shared" ca="1" si="3"/>
-        <v>99999780</v>
+        <v>99999049</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E024</v>
+        <v>5F5DD49</v>
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="5"/>
@@ -2317,17 +2317,17 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="6"/>
-        <v>99999780</v>
+        <v>99999049</v>
       </c>
     </row>
     <row r="39" spans="12:15">
       <c r="L39">
         <f t="shared" ca="1" si="3"/>
-        <v>99999334</v>
+        <v>99999038</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5DE66</v>
+        <v>5F5DD3E</v>
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="5"/>
@@ -2335,17 +2335,17 @@
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="6"/>
-        <v>99999334</v>
+        <v>99999038</v>
       </c>
     </row>
     <row r="40" spans="12:15">
       <c r="L40">
         <f t="shared" ca="1" si="3"/>
-        <v>99999818</v>
+        <v>99999580</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>5F5E04A</v>
+        <v>5F5DF5C</v>
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="5"/>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="6"/>
-        <v>99999818</v>
+        <v>99999580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>